<commit_message>
Update Global Reporting Attributes Catalog.xlsx
</commit_message>
<xml_diff>
--- a/docs/reporting/Global Reporting Attributes Catalog.xlsx
+++ b/docs/reporting/Global Reporting Attributes Catalog.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ASIAPAC.AD.JPMORGANCHASE.com\home2\APHOME10000\E881906\Saureen Adani\Modern Reporting Migrations &amp; Data\Reporting Attributes Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF14A23D-6000-413E-BE30-8C22F4482A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C199679-838E-4E82-A96A-13A264685772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B33461D6-A436-43CC-8683-934B3247E957}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="10950" xr2:uid="{B33461D6-A436-43CC-8683-934B3247E957}"/>
   </bookViews>
   <sheets>
-    <sheet name="Global Catalog - US, EU &amp; UK" sheetId="1" r:id="rId1"/>
+    <sheet name="Global Catalog - US,CAN,EU &amp; UK" sheetId="1" r:id="rId1"/>
     <sheet name="Global Catalog - AUS" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Global Catalog - AUS'!$D$5:$M$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Global Catalog - US, EU &amp; UK'!$D$5:$J$325</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Global Catalog - US,CAN,EU &amp; UK'!$D$5:$J$325</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3512,105 +3512,6 @@
   </si>
   <si>
     <t>Designates the hour, minute, seconds and date (if timestamp) or year, month, and date (if date) when the transaction (monetary or non-monetary) occurred.In this context, this is the timestamp of the transaction when the void was processed.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="26"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Reporting Attributes Catalog - US, EU &amp; UK Region </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="28"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Y =  Attribute available to use in Report Type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N =  Attribute not available to use in Report Type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Current Version: v2.0
-Last Updated: 08/21/2024
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: Historical data of upto last 6 months will be available for ad-hoc reporting</t>
-    </r>
   </si>
   <si>
     <r>
@@ -3713,6 +3614,95 @@
       <rPr>
         <i/>
         <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Historical data of upto last 6 months will be available for ad-hoc reporting</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reporting Attributes Catalog - US, CAN, EU &amp; UK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y =  Attribute available to use in Report Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N =  Attribute not available to use in Report Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Current Version: v2.0
+Last Updated: 08/22/2024
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -3900,10 +3890,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4467,7 +4457,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4484,14 +4474,14 @@
     <col min="10" max="10" width="26" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="14" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:10" s="14" customFormat="1" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:10" s="14" customFormat="1" ht="79.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:10" s="15" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="15" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:10" s="15" customFormat="1" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:10" s="15" customFormat="1" ht="79.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:10" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
@@ -14196,7 +14186,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14216,14 +14206,14 @@
     <col min="13" max="13" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="14" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:13" s="14" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:13" s="14" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:13" s="15" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="15" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:13" s="15" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:13" s="15" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
@@ -14264,7 +14254,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>624</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -14303,7 +14293,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>626</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -14342,7 +14332,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>628</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -14381,7 +14371,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>630</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -14420,7 +14410,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -14459,7 +14449,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>633</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -14498,7 +14488,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>635</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -14537,7 +14527,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -14576,7 +14566,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>637</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -14615,7 +14605,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>639</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -14654,7 +14644,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>641</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -14693,7 +14683,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>643</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -14732,7 +14722,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>644</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -14771,7 +14761,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>646</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -14810,7 +14800,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="9" t="s">
@@ -14849,7 +14839,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>649</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -14888,7 +14878,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>651</v>
       </c>
       <c r="B22" s="9" t="s">
@@ -14927,7 +14917,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>653</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -14966,7 +14956,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>655</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -15005,7 +14995,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>657</v>
       </c>
       <c r="B25" s="9" t="s">
@@ -15044,7 +15034,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="14" t="s">
         <v>658</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -15083,7 +15073,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>659</v>
       </c>
       <c r="B27" s="9" t="s">
@@ -15122,7 +15112,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="14" t="s">
         <v>660</v>
       </c>
       <c r="B28" s="9" t="s">
@@ -15161,7 +15151,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="14" t="s">
         <v>661</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -15200,7 +15190,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="14" t="s">
         <v>662</v>
       </c>
       <c r="B30" s="9" t="s">
@@ -15239,7 +15229,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="14" t="s">
         <v>663</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -15278,7 +15268,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="14" t="s">
         <v>664</v>
       </c>
       <c r="B32" s="9" t="s">
@@ -15317,7 +15307,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="14" t="s">
         <v>665</v>
       </c>
       <c r="B33" s="9" t="s">
@@ -15356,7 +15346,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="14" t="s">
         <v>667</v>
       </c>
       <c r="B34" s="9" t="s">
@@ -15395,7 +15385,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="14" t="s">
         <v>669</v>
       </c>
       <c r="B35" s="9" t="s">
@@ -15434,7 +15424,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="14" t="s">
         <v>671</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -15473,7 +15463,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="14" t="s">
         <v>673</v>
       </c>
       <c r="B37" s="9" t="s">
@@ -15512,7 +15502,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="14" t="s">
         <v>675</v>
       </c>
       <c r="B38" s="9" t="s">
@@ -15551,7 +15541,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="14" t="s">
         <v>677</v>
       </c>
       <c r="B39" s="9" t="s">
@@ -15590,7 +15580,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="14" t="s">
         <v>679</v>
       </c>
       <c r="B40" s="9" t="s">
@@ -15629,7 +15619,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="14" t="s">
         <v>681</v>
       </c>
       <c r="B41" s="9" t="s">
@@ -15668,7 +15658,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="14" t="s">
         <v>683</v>
       </c>
       <c r="B42" s="9" t="s">
@@ -15707,7 +15697,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="14" t="s">
         <v>685</v>
       </c>
       <c r="B43" s="9" t="s">
@@ -15746,7 +15736,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="14" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="9" t="s">
@@ -15785,7 +15775,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="14" t="s">
         <v>688</v>
       </c>
       <c r="B45" s="9" t="s">
@@ -15824,7 +15814,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="14" t="s">
         <v>689</v>
       </c>
       <c r="B46" s="9" t="s">
@@ -15863,7 +15853,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="14" t="s">
         <v>691</v>
       </c>
       <c r="B47" s="9" t="s">
@@ -15902,7 +15892,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="14" t="s">
         <v>693</v>
       </c>
       <c r="B48" s="9" t="s">
@@ -15941,7 +15931,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="14" t="s">
         <v>694</v>
       </c>
       <c r="B49" s="9" t="s">
@@ -15980,7 +15970,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="14" t="s">
         <v>696</v>
       </c>
       <c r="B50" s="9" t="s">
@@ -16019,7 +16009,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="14" t="s">
         <v>698</v>
       </c>
       <c r="B51" s="9" t="s">
@@ -16058,7 +16048,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="14" t="s">
         <v>699</v>
       </c>
       <c r="B52" s="9" t="s">
@@ -16097,7 +16087,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="14" t="s">
         <v>701</v>
       </c>
       <c r="B53" s="9" t="s">
@@ -16136,7 +16126,7 @@
       </c>
     </row>
     <row r="54" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="14" t="s">
         <v>703</v>
       </c>
       <c r="B54" s="9" t="s">
@@ -16175,7 +16165,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="14" t="s">
         <v>705</v>
       </c>
       <c r="B55" s="9" t="s">
@@ -16214,7 +16204,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="14" t="s">
         <v>707</v>
       </c>
       <c r="B56" s="9" t="s">
@@ -16253,7 +16243,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="14" t="s">
         <v>709</v>
       </c>
       <c r="B57" s="9" t="s">
@@ -16292,7 +16282,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="14" t="s">
         <v>711</v>
       </c>
       <c r="B58" s="9" t="s">
@@ -16331,7 +16321,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="14" t="s">
         <v>713</v>
       </c>
       <c r="B59" s="9" t="s">
@@ -16370,7 +16360,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="14" t="s">
         <v>715</v>
       </c>
       <c r="B60" s="9" t="s">
@@ -16409,7 +16399,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="15" t="s">
+      <c r="A61" s="14" t="s">
         <v>717</v>
       </c>
       <c r="B61" s="9" t="s">
@@ -16448,7 +16438,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="14" t="s">
         <v>719</v>
       </c>
       <c r="B62" s="9" t="s">
@@ -16487,7 +16477,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="15" t="s">
+      <c r="A63" s="14" t="s">
         <v>721</v>
       </c>
       <c r="B63" s="9" t="s">
@@ -16526,7 +16516,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
+      <c r="A64" s="14" t="s">
         <v>723</v>
       </c>
       <c r="B64" s="9" t="s">
@@ -16565,7 +16555,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="14" t="s">
         <v>725</v>
       </c>
       <c r="B65" s="9" t="s">
@@ -16604,7 +16594,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="15" t="s">
+      <c r="A66" s="14" t="s">
         <v>726</v>
       </c>
       <c r="B66" s="9" t="s">
@@ -16643,7 +16633,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="15" t="s">
+      <c r="A67" s="14" t="s">
         <v>728</v>
       </c>
       <c r="B67" s="9" t="s">
@@ -16682,7 +16672,7 @@
       </c>
     </row>
     <row r="68" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A68" s="15" t="s">
+      <c r="A68" s="14" t="s">
         <v>729</v>
       </c>
       <c r="B68" s="9" t="s">
@@ -16721,7 +16711,7 @@
       </c>
     </row>
     <row r="69" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
+      <c r="A69" s="14" t="s">
         <v>731</v>
       </c>
       <c r="B69" s="9" t="s">
@@ -16760,7 +16750,7 @@
       </c>
     </row>
     <row r="70" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="15" t="s">
+      <c r="A70" s="14" t="s">
         <v>733</v>
       </c>
       <c r="B70" s="9" t="s">
@@ -16799,7 +16789,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+      <c r="A71" s="14" t="s">
         <v>735</v>
       </c>
       <c r="B71" s="9" t="s">
@@ -16838,7 +16828,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
+      <c r="A72" s="14" t="s">
         <v>737</v>
       </c>
       <c r="B72" s="9" t="s">
@@ -16877,7 +16867,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
+      <c r="A73" s="14" t="s">
         <v>739</v>
       </c>
       <c r="B73" s="9" t="s">
@@ -16916,7 +16906,7 @@
       </c>
     </row>
     <row r="74" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
+      <c r="A74" s="14" t="s">
         <v>741</v>
       </c>
       <c r="B74" s="9" t="s">
@@ -16955,7 +16945,7 @@
       </c>
     </row>
     <row r="75" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
+      <c r="A75" s="14" t="s">
         <v>743</v>
       </c>
       <c r="B75" s="9" t="s">
@@ -16994,7 +16984,7 @@
       </c>
     </row>
     <row r="76" spans="1:13" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A76" s="15" t="s">
+      <c r="A76" s="14" t="s">
         <v>745</v>
       </c>
       <c r="B76" s="9" t="s">
@@ -17033,7 +17023,7 @@
       </c>
     </row>
     <row r="77" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
+      <c r="A77" s="14" t="s">
         <v>747</v>
       </c>
       <c r="B77" s="9" t="s">
@@ -17072,7 +17062,7 @@
       </c>
     </row>
     <row r="78" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" s="15" t="s">
+      <c r="A78" s="14" t="s">
         <v>749</v>
       </c>
       <c r="B78" s="9" t="s">
@@ -17111,7 +17101,7 @@
       </c>
     </row>
     <row r="79" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="14" t="s">
         <v>750</v>
       </c>
       <c r="B79" s="9" t="s">
@@ -17150,7 +17140,7 @@
       </c>
     </row>
     <row r="80" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A80" s="15" t="s">
+      <c r="A80" s="14" t="s">
         <v>752</v>
       </c>
       <c r="B80" s="9" t="s">
@@ -17189,7 +17179,7 @@
       </c>
     </row>
     <row r="81" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="15" t="s">
+      <c r="A81" s="14" t="s">
         <v>754</v>
       </c>
       <c r="B81" s="9" t="s">
@@ -17228,7 +17218,7 @@
       </c>
     </row>
     <row r="82" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="15" t="s">
+      <c r="A82" s="14" t="s">
         <v>756</v>
       </c>
       <c r="B82" s="9" t="s">
@@ -17267,7 +17257,7 @@
       </c>
     </row>
     <row r="83" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="15" t="s">
+      <c r="A83" s="14" t="s">
         <v>758</v>
       </c>
       <c r="B83" s="9" t="s">
@@ -17306,7 +17296,7 @@
       </c>
     </row>
     <row r="84" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="15" t="s">
+      <c r="A84" s="14" t="s">
         <v>760</v>
       </c>
       <c r="B84" s="9" t="s">
@@ -17345,7 +17335,7 @@
       </c>
     </row>
     <row r="85" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="15" t="s">
+      <c r="A85" s="14" t="s">
         <v>762</v>
       </c>
       <c r="B85" s="9" t="s">
@@ -17384,7 +17374,7 @@
       </c>
     </row>
     <row r="86" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="15" t="s">
+      <c r="A86" s="14" t="s">
         <v>764</v>
       </c>
       <c r="B86" s="9" t="s">
@@ -17423,7 +17413,7 @@
       </c>
     </row>
     <row r="87" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="15" t="s">
+      <c r="A87" s="14" t="s">
         <v>766</v>
       </c>
       <c r="B87" s="9" t="s">
@@ -17462,7 +17452,7 @@
       </c>
     </row>
     <row r="88" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="15" t="s">
+      <c r="A88" s="14" t="s">
         <v>768</v>
       </c>
       <c r="B88" s="9" t="s">
@@ -17501,7 +17491,7 @@
       </c>
     </row>
     <row r="89" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A89" s="15" t="s">
+      <c r="A89" s="14" t="s">
         <v>770</v>
       </c>
       <c r="B89" s="9" t="s">
@@ -17540,7 +17530,7 @@
       </c>
     </row>
     <row r="90" spans="1:13" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A90" s="15" t="s">
+      <c r="A90" s="14" t="s">
         <v>772</v>
       </c>
       <c r="B90" s="9" t="s">
@@ -17579,7 +17569,7 @@
       </c>
     </row>
     <row r="91" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="15" t="s">
+      <c r="A91" s="14" t="s">
         <v>774</v>
       </c>
       <c r="B91" s="9" t="s">
@@ -17618,7 +17608,7 @@
       </c>
     </row>
     <row r="92" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="15" t="s">
+      <c r="A92" s="14" t="s">
         <v>776</v>
       </c>
       <c r="B92" s="9" t="s">
@@ -17657,7 +17647,7 @@
       </c>
     </row>
     <row r="93" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A93" s="15" t="s">
+      <c r="A93" s="14" t="s">
         <v>778</v>
       </c>
       <c r="B93" s="9" t="s">
@@ -17696,7 +17686,7 @@
       </c>
     </row>
     <row r="94" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A94" s="15" t="s">
+      <c r="A94" s="14" t="s">
         <v>96</v>
       </c>
       <c r="B94" s="9" t="s">
@@ -17735,7 +17725,7 @@
       </c>
     </row>
     <row r="95" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="15" t="s">
+      <c r="A95" s="14" t="s">
         <v>780</v>
       </c>
       <c r="B95" s="9" t="s">
@@ -17774,7 +17764,7 @@
       </c>
     </row>
     <row r="96" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A96" s="15" t="s">
+      <c r="A96" s="14" t="s">
         <v>782</v>
       </c>
       <c r="B96" s="9" t="s">
@@ -17813,7 +17803,7 @@
       </c>
     </row>
     <row r="97" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A97" s="15" t="s">
+      <c r="A97" s="14" t="s">
         <v>784</v>
       </c>
       <c r="B97" s="9" t="s">
@@ -17852,7 +17842,7 @@
       </c>
     </row>
     <row r="98" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="15" t="s">
+      <c r="A98" s="14" t="s">
         <v>786</v>
       </c>
       <c r="B98" s="9" t="s">
@@ -17891,7 +17881,7 @@
       </c>
     </row>
     <row r="99" spans="1:13" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A99" s="15" t="s">
+      <c r="A99" s="14" t="s">
         <v>787</v>
       </c>
       <c r="B99" s="9" t="s">
@@ -17930,7 +17920,7 @@
       </c>
     </row>
     <row r="100" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A100" s="15" t="s">
+      <c r="A100" s="14" t="s">
         <v>102</v>
       </c>
       <c r="B100" s="9" t="s">
@@ -17969,7 +17959,7 @@
       </c>
     </row>
     <row r="101" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A101" s="15" t="s">
+      <c r="A101" s="14" t="s">
         <v>790</v>
       </c>
       <c r="B101" s="9" t="s">
@@ -18008,7 +17998,7 @@
       </c>
     </row>
     <row r="102" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="15" t="s">
+      <c r="A102" s="14" t="s">
         <v>792</v>
       </c>
       <c r="B102" s="9" t="s">
@@ -18047,7 +18037,7 @@
       </c>
     </row>
     <row r="103" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A103" s="15" t="s">
+      <c r="A103" s="14" t="s">
         <v>794</v>
       </c>
       <c r="B103" s="9" t="s">
@@ -18086,7 +18076,7 @@
       </c>
     </row>
     <row r="104" spans="1:13" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A104" s="15" t="s">
+      <c r="A104" s="14" t="s">
         <v>796</v>
       </c>
       <c r="B104" s="9" t="s">
@@ -18125,7 +18115,7 @@
       </c>
     </row>
     <row r="105" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A105" s="15" t="s">
+      <c r="A105" s="14" t="s">
         <v>798</v>
       </c>
       <c r="B105" s="9" t="s">
@@ -18164,7 +18154,7 @@
       </c>
     </row>
     <row r="106" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A106" s="15" t="s">
+      <c r="A106" s="14" t="s">
         <v>800</v>
       </c>
       <c r="B106" s="9" t="s">
@@ -18203,7 +18193,7 @@
       </c>
     </row>
     <row r="107" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A107" s="15" t="s">
+      <c r="A107" s="14" t="s">
         <v>802</v>
       </c>
       <c r="B107" s="9" t="s">
@@ -18242,7 +18232,7 @@
       </c>
     </row>
     <row r="108" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A108" s="15" t="s">
+      <c r="A108" s="14" t="s">
         <v>804</v>
       </c>
       <c r="B108" s="9" t="s">
@@ -18281,7 +18271,7 @@
       </c>
     </row>
     <row r="109" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="15" t="s">
+      <c r="A109" s="14" t="s">
         <v>806</v>
       </c>
       <c r="B109" s="9" t="s">
@@ -18320,7 +18310,7 @@
       </c>
     </row>
     <row r="110" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="15" t="s">
+      <c r="A110" s="14" t="s">
         <v>808</v>
       </c>
       <c r="B110" s="9" t="s">
@@ -18359,7 +18349,7 @@
       </c>
     </row>
     <row r="111" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="15" t="s">
+      <c r="A111" s="14" t="s">
         <v>810</v>
       </c>
       <c r="B111" s="9" t="s">
@@ -18398,7 +18388,7 @@
       </c>
     </row>
     <row r="112" spans="1:13" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A112" s="15" t="s">
+      <c r="A112" s="14" t="s">
         <v>812</v>
       </c>
       <c r="B112" s="9" t="s">
@@ -18437,7 +18427,7 @@
       </c>
     </row>
     <row r="113" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A113" s="15" t="s">
+      <c r="A113" s="14" t="s">
         <v>814</v>
       </c>
       <c r="B113" s="9" t="s">
@@ -18476,7 +18466,7 @@
       </c>
     </row>
     <row r="114" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A114" s="15" t="s">
+      <c r="A114" s="14" t="s">
         <v>816</v>
       </c>
       <c r="B114" s="9" t="s">
@@ -18515,7 +18505,7 @@
       </c>
     </row>
     <row r="115" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="15" t="s">
+      <c r="A115" s="14" t="s">
         <v>818</v>
       </c>
       <c r="B115" s="9" t="s">
@@ -18554,7 +18544,7 @@
       </c>
     </row>
     <row r="116" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A116" s="15" t="s">
+      <c r="A116" s="14" t="s">
         <v>820</v>
       </c>
       <c r="B116" s="9" t="s">
@@ -18593,7 +18583,7 @@
       </c>
     </row>
     <row r="117" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="15" t="s">
+      <c r="A117" s="14" t="s">
         <v>822</v>
       </c>
       <c r="B117" s="9" t="s">
@@ -18632,7 +18622,7 @@
       </c>
     </row>
     <row r="118" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A118" s="15" t="s">
+      <c r="A118" s="14" t="s">
         <v>824</v>
       </c>
       <c r="B118" s="9" t="s">
@@ -18671,7 +18661,7 @@
       </c>
     </row>
     <row r="119" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A119" s="15" t="s">
+      <c r="A119" s="14" t="s">
         <v>826</v>
       </c>
       <c r="B119" s="9" t="s">
@@ -18710,7 +18700,7 @@
       </c>
     </row>
     <row r="120" spans="1:13" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A120" s="15" t="s">
+      <c r="A120" s="14" t="s">
         <v>828</v>
       </c>
       <c r="B120" s="9" t="s">
@@ -18749,7 +18739,7 @@
       </c>
     </row>
     <row r="121" spans="1:13" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A121" s="15" t="s">
+      <c r="A121" s="14" t="s">
         <v>119</v>
       </c>
       <c r="B121" s="9" t="s">
@@ -18788,7 +18778,7 @@
       </c>
     </row>
     <row r="122" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A122" s="15" t="s">
+      <c r="A122" s="14" t="s">
         <v>831</v>
       </c>
       <c r="B122" s="9" t="s">
@@ -18827,7 +18817,7 @@
       </c>
     </row>
     <row r="123" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A123" s="15" t="s">
+      <c r="A123" s="14" t="s">
         <v>833</v>
       </c>
       <c r="B123" s="9" t="s">
@@ -18866,7 +18856,7 @@
       </c>
     </row>
     <row r="124" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A124" s="15" t="s">
+      <c r="A124" s="14" t="s">
         <v>835</v>
       </c>
       <c r="B124" s="9" t="s">
@@ -18905,7 +18895,7 @@
       </c>
     </row>
     <row r="125" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="15" t="s">
+      <c r="A125" s="14" t="s">
         <v>837</v>
       </c>
       <c r="B125" s="9" t="s">
@@ -18944,7 +18934,7 @@
       </c>
     </row>
     <row r="126" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A126" s="15" t="s">
+      <c r="A126" s="14" t="s">
         <v>839</v>
       </c>
       <c r="B126" s="9" t="s">
@@ -18983,7 +18973,7 @@
       </c>
     </row>
     <row r="127" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A127" s="15" t="s">
+      <c r="A127" s="14" t="s">
         <v>126</v>
       </c>
       <c r="B127" s="9" t="s">
@@ -19022,7 +19012,7 @@
       </c>
     </row>
     <row r="128" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A128" s="15" t="s">
+      <c r="A128" s="14" t="s">
         <v>841</v>
       </c>
       <c r="B128" s="9" t="s">
@@ -19061,7 +19051,7 @@
       </c>
     </row>
     <row r="129" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A129" s="15" t="s">
+      <c r="A129" s="14" t="s">
         <v>843</v>
       </c>
       <c r="B129" s="9" t="s">
@@ -19100,7 +19090,7 @@
       </c>
     </row>
     <row r="130" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A130" s="15" t="s">
+      <c r="A130" s="14" t="s">
         <v>845</v>
       </c>
       <c r="B130" s="9" t="s">
@@ -19139,7 +19129,7 @@
       </c>
     </row>
     <row r="131" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A131" s="15" t="s">
+      <c r="A131" s="14" t="s">
         <v>847</v>
       </c>
       <c r="B131" s="9" t="s">
@@ -19178,7 +19168,7 @@
       </c>
     </row>
     <row r="132" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A132" s="15" t="s">
+      <c r="A132" s="14" t="s">
         <v>849</v>
       </c>
       <c r="B132" s="9" t="s">
@@ -19217,7 +19207,7 @@
       </c>
     </row>
     <row r="133" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A133" s="15" t="s">
+      <c r="A133" s="14" t="s">
         <v>851</v>
       </c>
       <c r="B133" s="9" t="s">
@@ -19256,7 +19246,7 @@
       </c>
     </row>
     <row r="134" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A134" s="15" t="s">
+      <c r="A134" s="14" t="s">
         <v>853</v>
       </c>
       <c r="B134" s="9" t="s">
@@ -19295,7 +19285,7 @@
       </c>
     </row>
     <row r="135" spans="1:13" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A135" s="15" t="s">
+      <c r="A135" s="14" t="s">
         <v>855</v>
       </c>
       <c r="B135" s="9" t="s">
@@ -19334,7 +19324,7 @@
       </c>
     </row>
     <row r="136" spans="1:13" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A136" s="15" t="s">
+      <c r="A136" s="14" t="s">
         <v>857</v>
       </c>
       <c r="B136" s="9" t="s">
@@ -19373,7 +19363,7 @@
       </c>
     </row>
     <row r="137" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A137" s="15" t="s">
+      <c r="A137" s="14" t="s">
         <v>859</v>
       </c>
       <c r="B137" s="9" t="s">
@@ -19412,7 +19402,7 @@
       </c>
     </row>
     <row r="138" spans="1:13" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A138" s="15" t="s">
+      <c r="A138" s="14" t="s">
         <v>861</v>
       </c>
       <c r="B138" s="9" t="s">
@@ -19451,7 +19441,7 @@
       </c>
     </row>
     <row r="139" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A139" s="15" t="s">
+      <c r="A139" s="14" t="s">
         <v>863</v>
       </c>
       <c r="B139" s="9" t="s">
@@ -19490,7 +19480,7 @@
       </c>
     </row>
     <row r="140" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A140" s="15" t="s">
+      <c r="A140" s="14" t="s">
         <v>865</v>
       </c>
       <c r="B140" s="9" t="s">
@@ -19529,7 +19519,7 @@
       </c>
     </row>
     <row r="141" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A141" s="15" t="s">
+      <c r="A141" s="14" t="s">
         <v>867</v>
       </c>
       <c r="B141" s="9" t="s">
@@ -19568,7 +19558,7 @@
       </c>
     </row>
     <row r="142" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A142" s="15" t="s">
+      <c r="A142" s="14" t="s">
         <v>868</v>
       </c>
       <c r="B142" s="9" t="s">
@@ -19607,7 +19597,7 @@
       </c>
     </row>
     <row r="143" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A143" s="15" t="s">
+      <c r="A143" s="14" t="s">
         <v>869</v>
       </c>
       <c r="B143" s="9" t="s">
@@ -19646,7 +19636,7 @@
       </c>
     </row>
     <row r="144" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A144" s="15" t="s">
+      <c r="A144" s="14" t="s">
         <v>870</v>
       </c>
       <c r="B144" s="9" t="s">
@@ -19685,7 +19675,7 @@
       </c>
     </row>
     <row r="145" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A145" s="15" t="s">
+      <c r="A145" s="14" t="s">
         <v>872</v>
       </c>
       <c r="B145" s="9" t="s">
@@ -19724,7 +19714,7 @@
       </c>
     </row>
     <row r="146" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A146" s="15" t="s">
+      <c r="A146" s="14" t="s">
         <v>144</v>
       </c>
       <c r="B146" s="9" t="s">
@@ -19763,7 +19753,7 @@
       </c>
     </row>
     <row r="147" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A147" s="15" t="s">
+      <c r="A147" s="14" t="s">
         <v>874</v>
       </c>
       <c r="B147" s="9" t="s">
@@ -19802,7 +19792,7 @@
       </c>
     </row>
     <row r="148" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="15" t="s">
+      <c r="A148" s="14" t="s">
         <v>876</v>
       </c>
       <c r="B148" s="9" t="s">
@@ -19841,7 +19831,7 @@
       </c>
     </row>
     <row r="149" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A149" s="15" t="s">
+      <c r="A149" s="14" t="s">
         <v>878</v>
       </c>
       <c r="B149" s="9" t="s">
@@ -19880,7 +19870,7 @@
       </c>
     </row>
     <row r="150" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A150" s="15" t="s">
+      <c r="A150" s="14" t="s">
         <v>880</v>
       </c>
       <c r="B150" s="9" t="s">
@@ -19919,7 +19909,7 @@
       </c>
     </row>
     <row r="151" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A151" s="15" t="s">
+      <c r="A151" s="14" t="s">
         <v>882</v>
       </c>
       <c r="B151" s="9" t="s">
@@ -19958,7 +19948,7 @@
       </c>
     </row>
     <row r="152" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A152" s="15" t="s">
+      <c r="A152" s="14" t="s">
         <v>884</v>
       </c>
       <c r="B152" s="9" t="s">
@@ -19997,7 +19987,7 @@
       </c>
     </row>
     <row r="153" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A153" s="15" t="s">
+      <c r="A153" s="14" t="s">
         <v>886</v>
       </c>
       <c r="B153" s="9" t="s">
@@ -20036,7 +20026,7 @@
       </c>
     </row>
     <row r="154" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="15" t="s">
+      <c r="A154" s="14" t="s">
         <v>888</v>
       </c>
       <c r="B154" s="9" t="s">
@@ -20075,7 +20065,7 @@
       </c>
     </row>
     <row r="155" spans="1:13" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A155" s="15" t="s">
+      <c r="A155" s="14" t="s">
         <v>890</v>
       </c>
       <c r="B155" s="9" t="s">
@@ -20114,7 +20104,7 @@
       </c>
     </row>
     <row r="156" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A156" s="15" t="s">
+      <c r="A156" s="14" t="s">
         <v>892</v>
       </c>
       <c r="B156" s="9" t="s">
@@ -20153,7 +20143,7 @@
       </c>
     </row>
     <row r="157" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A157" s="15" t="s">
+      <c r="A157" s="14" t="s">
         <v>147</v>
       </c>
       <c r="B157" s="9" t="s">
@@ -20192,7 +20182,7 @@
       </c>
     </row>
     <row r="158" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A158" s="15" t="s">
+      <c r="A158" s="14" t="s">
         <v>895</v>
       </c>
       <c r="B158" s="9" t="s">
@@ -20231,7 +20221,7 @@
       </c>
     </row>
     <row r="159" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A159" s="15" t="s">
+      <c r="A159" s="14" t="s">
         <v>897</v>
       </c>
       <c r="B159" s="9" t="s">
@@ -20270,7 +20260,7 @@
       </c>
     </row>
     <row r="160" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A160" s="15" t="s">
+      <c r="A160" s="14" t="s">
         <v>898</v>
       </c>
       <c r="B160" s="9" t="s">
@@ -20309,7 +20299,7 @@
       </c>
     </row>
     <row r="161" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A161" s="15" t="s">
+      <c r="A161" s="14" t="s">
         <v>900</v>
       </c>
       <c r="B161" s="9" t="s">
@@ -20348,7 +20338,7 @@
       </c>
     </row>
     <row r="162" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" s="15" t="s">
+      <c r="A162" s="14" t="s">
         <v>901</v>
       </c>
       <c r="B162" s="9" t="s">
@@ -20387,7 +20377,7 @@
       </c>
     </row>
     <row r="163" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A163" s="15" t="s">
+      <c r="A163" s="14" t="s">
         <v>902</v>
       </c>
       <c r="B163" s="9" t="s">
@@ -20426,7 +20416,7 @@
       </c>
     </row>
     <row r="164" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A164" s="15" t="s">
+      <c r="A164" s="14" t="s">
         <v>904</v>
       </c>
       <c r="B164" s="9" t="s">
@@ -20465,7 +20455,7 @@
       </c>
     </row>
     <row r="165" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A165" s="15" t="s">
+      <c r="A165" s="14" t="s">
         <v>906</v>
       </c>
       <c r="B165" s="9" t="s">
@@ -20504,7 +20494,7 @@
       </c>
     </row>
     <row r="166" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A166" s="15" t="s">
+      <c r="A166" s="14" t="s">
         <v>908</v>
       </c>
       <c r="B166" s="9" t="s">
@@ -20543,7 +20533,7 @@
       </c>
     </row>
     <row r="167" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A167" s="15" t="s">
+      <c r="A167" s="14" t="s">
         <v>910</v>
       </c>
       <c r="B167" s="9" t="s">
@@ -20582,7 +20572,7 @@
       </c>
     </row>
     <row r="168" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A168" s="15" t="s">
+      <c r="A168" s="14" t="s">
         <v>912</v>
       </c>
       <c r="B168" s="9" t="s">
@@ -20621,7 +20611,7 @@
       </c>
     </row>
     <row r="169" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A169" s="15" t="s">
+      <c r="A169" s="14" t="s">
         <v>914</v>
       </c>
       <c r="B169" s="9" t="s">
@@ -20660,7 +20650,7 @@
       </c>
     </row>
     <row r="170" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A170" s="15" t="s">
+      <c r="A170" s="14" t="s">
         <v>916</v>
       </c>
       <c r="B170" s="9" t="s">
@@ -20699,7 +20689,7 @@
       </c>
     </row>
     <row r="171" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A171" s="15" t="s">
+      <c r="A171" s="14" t="s">
         <v>918</v>
       </c>
       <c r="B171" s="9" t="s">
@@ -20738,7 +20728,7 @@
       </c>
     </row>
     <row r="172" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A172" s="15" t="s">
+      <c r="A172" s="14" t="s">
         <v>920</v>
       </c>
       <c r="B172" s="9" t="s">
@@ -20777,7 +20767,7 @@
       </c>
     </row>
     <row r="173" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="15" t="s">
+      <c r="A173" s="14" t="s">
         <v>922</v>
       </c>
       <c r="B173" s="9" t="s">
@@ -20816,7 +20806,7 @@
       </c>
     </row>
     <row r="174" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A174" s="15" t="s">
+      <c r="A174" s="14" t="s">
         <v>924</v>
       </c>
       <c r="B174" s="9" t="s">
@@ -20855,7 +20845,7 @@
       </c>
     </row>
     <row r="175" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A175" s="15" t="s">
+      <c r="A175" s="14" t="s">
         <v>157</v>
       </c>
       <c r="B175" s="9" t="s">
@@ -20894,7 +20884,7 @@
       </c>
     </row>
     <row r="176" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A176" s="15" t="s">
+      <c r="A176" s="14" t="s">
         <v>927</v>
       </c>
       <c r="B176" s="9" t="s">
@@ -20933,7 +20923,7 @@
       </c>
     </row>
     <row r="177" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A177" s="15" t="s">
+      <c r="A177" s="14" t="s">
         <v>929</v>
       </c>
       <c r="B177" s="9" t="s">
@@ -20972,7 +20962,7 @@
       </c>
     </row>
     <row r="178" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A178" s="15" t="s">
+      <c r="A178" s="14" t="s">
         <v>931</v>
       </c>
       <c r="B178" s="9" t="s">
@@ -21011,7 +21001,7 @@
       </c>
     </row>
     <row r="179" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A179" s="15" t="s">
+      <c r="A179" s="14" t="s">
         <v>933</v>
       </c>
       <c r="B179" s="9" t="s">
@@ -21050,7 +21040,7 @@
       </c>
     </row>
     <row r="180" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A180" s="15" t="s">
+      <c r="A180" s="14" t="s">
         <v>935</v>
       </c>
       <c r="B180" s="9" t="s">
@@ -21089,7 +21079,7 @@
       </c>
     </row>
     <row r="181" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A181" s="15" t="s">
+      <c r="A181" s="14" t="s">
         <v>936</v>
       </c>
       <c r="B181" s="9" t="s">
@@ -21128,7 +21118,7 @@
       </c>
     </row>
     <row r="182" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A182" s="15" t="s">
+      <c r="A182" s="14" t="s">
         <v>938</v>
       </c>
       <c r="B182" s="9" t="s">
@@ -21167,7 +21157,7 @@
       </c>
     </row>
     <row r="183" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A183" s="15" t="s">
+      <c r="A183" s="14" t="s">
         <v>940</v>
       </c>
       <c r="B183" s="9" t="s">
@@ -21206,7 +21196,7 @@
       </c>
     </row>
     <row r="184" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A184" s="15" t="s">
+      <c r="A184" s="14" t="s">
         <v>942</v>
       </c>
       <c r="B184" s="9" t="s">
@@ -21245,7 +21235,7 @@
       </c>
     </row>
     <row r="185" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A185" s="15" t="s">
+      <c r="A185" s="14" t="s">
         <v>944</v>
       </c>
       <c r="B185" s="9" t="s">
@@ -21284,7 +21274,7 @@
       </c>
     </row>
     <row r="186" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A186" s="15" t="s">
+      <c r="A186" s="14" t="s">
         <v>162</v>
       </c>
       <c r="B186" s="9" t="s">
@@ -21323,7 +21313,7 @@
       </c>
     </row>
     <row r="187" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A187" s="15" t="s">
+      <c r="A187" s="14" t="s">
         <v>946</v>
       </c>
       <c r="B187" s="9" t="s">
@@ -21362,7 +21352,7 @@
       </c>
     </row>
     <row r="188" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A188" s="15" t="s">
+      <c r="A188" s="14" t="s">
         <v>948</v>
       </c>
       <c r="B188" s="9" t="s">
@@ -21401,7 +21391,7 @@
       </c>
     </row>
     <row r="189" spans="1:13" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A189" s="15" t="s">
+      <c r="A189" s="14" t="s">
         <v>950</v>
       </c>
       <c r="B189" s="9" t="s">
@@ -21440,7 +21430,7 @@
       </c>
     </row>
     <row r="190" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A190" s="15" t="s">
+      <c r="A190" s="14" t="s">
         <v>952</v>
       </c>
       <c r="B190" s="9" t="s">
@@ -21479,7 +21469,7 @@
       </c>
     </row>
     <row r="191" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A191" s="15" t="s">
+      <c r="A191" s="14" t="s">
         <v>954</v>
       </c>
       <c r="B191" s="9" t="s">
@@ -21518,7 +21508,7 @@
       </c>
     </row>
     <row r="192" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A192" s="15" t="s">
+      <c r="A192" s="14" t="s">
         <v>956</v>
       </c>
       <c r="B192" s="9" t="s">
@@ -21557,7 +21547,7 @@
       </c>
     </row>
     <row r="193" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A193" s="15" t="s">
+      <c r="A193" s="14" t="s">
         <v>958</v>
       </c>
       <c r="B193" s="9" t="s">
@@ -21596,7 +21586,7 @@
       </c>
     </row>
     <row r="194" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A194" s="15" t="s">
+      <c r="A194" s="14" t="s">
         <v>960</v>
       </c>
       <c r="B194" s="9" t="s">
@@ -21635,7 +21625,7 @@
       </c>
     </row>
     <row r="195" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A195" s="15" t="s">
+      <c r="A195" s="14" t="s">
         <v>962</v>
       </c>
       <c r="B195" s="9" t="s">
@@ -21674,7 +21664,7 @@
       </c>
     </row>
     <row r="196" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A196" s="15" t="s">
+      <c r="A196" s="14" t="s">
         <v>964</v>
       </c>
       <c r="B196" s="9" t="s">
@@ -21713,7 +21703,7 @@
       </c>
     </row>
     <row r="197" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A197" s="15" t="s">
+      <c r="A197" s="14" t="s">
         <v>966</v>
       </c>
       <c r="B197" s="9" t="s">
@@ -21752,7 +21742,7 @@
       </c>
     </row>
     <row r="198" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A198" s="15" t="s">
+      <c r="A198" s="14" t="s">
         <v>968</v>
       </c>
       <c r="B198" s="9" t="s">
@@ -21791,7 +21781,7 @@
       </c>
     </row>
     <row r="199" spans="1:13" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A199" s="15" t="s">
+      <c r="A199" s="14" t="s">
         <v>970</v>
       </c>
       <c r="B199" s="9" t="s">
@@ -21830,7 +21820,7 @@
       </c>
     </row>
     <row r="200" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A200" s="15" t="s">
+      <c r="A200" s="14" t="s">
         <v>972</v>
       </c>
       <c r="B200" s="9" t="s">
@@ -21869,7 +21859,7 @@
       </c>
     </row>
     <row r="201" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A201" s="15" t="s">
+      <c r="A201" s="14" t="s">
         <v>974</v>
       </c>
       <c r="B201" s="9" t="s">
@@ -21908,7 +21898,7 @@
       </c>
     </row>
     <row r="202" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A202" s="15" t="s">
+      <c r="A202" s="14" t="s">
         <v>976</v>
       </c>
       <c r="B202" s="9" t="s">
@@ -21947,7 +21937,7 @@
       </c>
     </row>
     <row r="203" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A203" s="15" t="s">
+      <c r="A203" s="14" t="s">
         <v>977</v>
       </c>
       <c r="B203" s="9" t="s">
@@ -21986,7 +21976,7 @@
       </c>
     </row>
     <row r="204" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A204" s="15" t="s">
+      <c r="A204" s="14" t="s">
         <v>979</v>
       </c>
       <c r="B204" s="9" t="s">
@@ -22025,7 +22015,7 @@
       </c>
     </row>
     <row r="205" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A205" s="15" t="s">
+      <c r="A205" s="14" t="s">
         <v>981</v>
       </c>
       <c r="B205" s="9" t="s">
@@ -22064,7 +22054,7 @@
       </c>
     </row>
     <row r="206" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A206" s="15" t="s">
+      <c r="A206" s="14" t="s">
         <v>983</v>
       </c>
       <c r="B206" s="9" t="s">
@@ -22103,7 +22093,7 @@
       </c>
     </row>
     <row r="207" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A207" s="15" t="s">
+      <c r="A207" s="14" t="s">
         <v>985</v>
       </c>
       <c r="B207" s="9" t="s">
@@ -22142,7 +22132,7 @@
       </c>
     </row>
     <row r="208" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A208" s="15" t="s">
+      <c r="A208" s="14" t="s">
         <v>987</v>
       </c>
       <c r="B208" s="9" t="s">
@@ -22181,7 +22171,7 @@
       </c>
     </row>
     <row r="209" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A209" s="15" t="s">
+      <c r="A209" s="14" t="s">
         <v>989</v>
       </c>
       <c r="B209" s="9" t="s">
@@ -22220,7 +22210,7 @@
       </c>
     </row>
     <row r="210" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A210" s="15" t="s">
+      <c r="A210" s="14" t="s">
         <v>991</v>
       </c>
       <c r="B210" s="9" t="s">
@@ -22259,7 +22249,7 @@
       </c>
     </row>
     <row r="211" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A211" s="15" t="s">
+      <c r="A211" s="14" t="s">
         <v>993</v>
       </c>
       <c r="B211" s="9" t="s">
@@ -22298,7 +22288,7 @@
       </c>
     </row>
     <row r="212" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A212" s="15" t="s">
+      <c r="A212" s="14" t="s">
         <v>995</v>
       </c>
       <c r="B212" s="9" t="s">
@@ -22337,7 +22327,7 @@
       </c>
     </row>
     <row r="213" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A213" s="15" t="s">
+      <c r="A213" s="14" t="s">
         <v>997</v>
       </c>
       <c r="B213" s="9" t="s">
@@ -22376,7 +22366,7 @@
       </c>
     </row>
     <row r="214" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A214" s="15" t="s">
+      <c r="A214" s="14" t="s">
         <v>999</v>
       </c>
       <c r="B214" s="9" t="s">
@@ -22415,7 +22405,7 @@
       </c>
     </row>
     <row r="215" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A215" s="15" t="s">
+      <c r="A215" s="14" t="s">
         <v>183</v>
       </c>
       <c r="B215" s="9" t="s">
@@ -22454,7 +22444,7 @@
       </c>
     </row>
     <row r="216" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A216" s="15" t="s">
+      <c r="A216" s="14" t="s">
         <v>1002</v>
       </c>
       <c r="B216" s="9" t="s">
@@ -22493,7 +22483,7 @@
       </c>
     </row>
     <row r="217" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A217" s="15" t="s">
+      <c r="A217" s="14" t="s">
         <v>1004</v>
       </c>
       <c r="B217" s="9" t="s">
@@ -22532,7 +22522,7 @@
       </c>
     </row>
     <row r="218" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A218" s="15" t="s">
+      <c r="A218" s="14" t="s">
         <v>1006</v>
       </c>
       <c r="B218" s="9" t="s">
@@ -22571,7 +22561,7 @@
       </c>
     </row>
     <row r="219" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A219" s="15" t="s">
+      <c r="A219" s="14" t="s">
         <v>1008</v>
       </c>
       <c r="B219" s="9" t="s">
@@ -22610,7 +22600,7 @@
       </c>
     </row>
     <row r="220" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A220" s="15" t="s">
+      <c r="A220" s="14" t="s">
         <v>1010</v>
       </c>
       <c r="B220" s="9" t="s">
@@ -22649,7 +22639,7 @@
       </c>
     </row>
     <row r="221" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A221" s="15" t="s">
+      <c r="A221" s="14" t="s">
         <v>1011</v>
       </c>
       <c r="B221" s="9" t="s">
@@ -22688,7 +22678,7 @@
       </c>
     </row>
     <row r="222" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A222" s="15" t="s">
+      <c r="A222" s="14" t="s">
         <v>1013</v>
       </c>
       <c r="B222" s="9" t="s">
@@ -22727,7 +22717,7 @@
       </c>
     </row>
     <row r="223" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A223" s="15" t="s">
+      <c r="A223" s="14" t="s">
         <v>1015</v>
       </c>
       <c r="B223" s="9" t="s">
@@ -22766,7 +22756,7 @@
       </c>
     </row>
     <row r="224" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A224" s="15" t="s">
+      <c r="A224" s="14" t="s">
         <v>1017</v>
       </c>
       <c r="B224" s="9" t="s">
@@ -22805,7 +22795,7 @@
       </c>
     </row>
     <row r="225" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A225" s="15" t="s">
+      <c r="A225" s="14" t="s">
         <v>1019</v>
       </c>
       <c r="B225" s="9" t="s">
@@ -22844,7 +22834,7 @@
       </c>
     </row>
     <row r="226" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A226" s="15" t="s">
+      <c r="A226" s="14" t="s">
         <v>1021</v>
       </c>
       <c r="B226" s="9" t="s">
@@ -22883,7 +22873,7 @@
       </c>
     </row>
     <row r="227" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A227" s="15" t="s">
+      <c r="A227" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="B227" s="9" t="s">
@@ -22922,7 +22912,7 @@
       </c>
     </row>
     <row r="228" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A228" s="15" t="s">
+      <c r="A228" s="14" t="s">
         <v>1025</v>
       </c>
       <c r="B228" s="9" t="s">
@@ -22961,7 +22951,7 @@
       </c>
     </row>
     <row r="229" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A229" s="15" t="s">
+      <c r="A229" s="14" t="s">
         <v>1027</v>
       </c>
       <c r="B229" s="9" t="s">
@@ -23000,7 +22990,7 @@
       </c>
     </row>
     <row r="230" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A230" s="15" t="s">
+      <c r="A230" s="14" t="s">
         <v>1029</v>
       </c>
       <c r="B230" s="9" t="s">
@@ -23039,7 +23029,7 @@
       </c>
     </row>
     <row r="231" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A231" s="15" t="s">
+      <c r="A231" s="14" t="s">
         <v>1031</v>
       </c>
       <c r="B231" s="9" t="s">
@@ -23078,7 +23068,7 @@
       </c>
     </row>
     <row r="232" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A232" s="15" t="s">
+      <c r="A232" s="14" t="s">
         <v>1033</v>
       </c>
       <c r="B232" s="9" t="s">
@@ -23117,7 +23107,7 @@
       </c>
     </row>
     <row r="233" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A233" s="15" t="s">
+      <c r="A233" s="14" t="s">
         <v>1035</v>
       </c>
       <c r="B233" s="9" t="s">
@@ -23156,7 +23146,7 @@
       </c>
     </row>
     <row r="234" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A234" s="15" t="s">
+      <c r="A234" s="14" t="s">
         <v>1037</v>
       </c>
       <c r="B234" s="9" t="s">
@@ -23195,7 +23185,7 @@
       </c>
     </row>
     <row r="235" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A235" s="15" t="s">
+      <c r="A235" s="14" t="s">
         <v>1039</v>
       </c>
       <c r="B235" s="9" t="s">
@@ -23234,7 +23224,7 @@
       </c>
     </row>
     <row r="236" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A236" s="15" t="s">
+      <c r="A236" s="14" t="s">
         <v>1041</v>
       </c>
       <c r="B236" s="9" t="s">
@@ -23273,7 +23263,7 @@
       </c>
     </row>
     <row r="237" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A237" s="15" t="s">
+      <c r="A237" s="14" t="s">
         <v>1043</v>
       </c>
       <c r="B237" s="9" t="s">
@@ -23312,7 +23302,7 @@
       </c>
     </row>
     <row r="238" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A238" s="15" t="s">
+      <c r="A238" s="14" t="s">
         <v>1044</v>
       </c>
       <c r="B238" s="9" t="s">
@@ -23351,7 +23341,7 @@
       </c>
     </row>
     <row r="239" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A239" s="15" t="s">
+      <c r="A239" s="14" t="s">
         <v>1045</v>
       </c>
       <c r="B239" s="9" t="s">
@@ -23390,7 +23380,7 @@
       </c>
     </row>
     <row r="240" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A240" s="15" t="s">
+      <c r="A240" s="14" t="s">
         <v>1047</v>
       </c>
       <c r="B240" s="9" t="s">
@@ -23429,7 +23419,7 @@
       </c>
     </row>
     <row r="241" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A241" s="15" t="s">
+      <c r="A241" s="14" t="s">
         <v>1048</v>
       </c>
       <c r="B241" s="9" t="s">
@@ -23468,7 +23458,7 @@
       </c>
     </row>
     <row r="242" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A242" s="15" t="s">
+      <c r="A242" s="14" t="s">
         <v>1049</v>
       </c>
       <c r="B242" s="9" t="s">
@@ -23507,7 +23497,7 @@
       </c>
     </row>
     <row r="243" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A243" s="15" t="s">
+      <c r="A243" s="14" t="s">
         <v>1050</v>
       </c>
       <c r="B243" s="9" t="s">
@@ -23546,7 +23536,7 @@
       </c>
     </row>
     <row r="244" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A244" s="15" t="s">
+      <c r="A244" s="14" t="s">
         <v>1051</v>
       </c>
       <c r="B244" s="9" t="s">
@@ -23585,7 +23575,7 @@
       </c>
     </row>
     <row r="245" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A245" s="15" t="s">
+      <c r="A245" s="14" t="s">
         <v>1052</v>
       </c>
       <c r="B245" s="9" t="s">
@@ -23624,7 +23614,7 @@
       </c>
     </row>
     <row r="246" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A246" s="15" t="s">
+      <c r="A246" s="14" t="s">
         <v>1053</v>
       </c>
       <c r="B246" s="9" t="s">
@@ -23663,7 +23653,7 @@
       </c>
     </row>
     <row r="247" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A247" s="15" t="s">
+      <c r="A247" s="14" t="s">
         <v>1054</v>
       </c>
       <c r="B247" s="9" t="s">
@@ -23702,7 +23692,7 @@
       </c>
     </row>
     <row r="248" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A248" s="15" t="s">
+      <c r="A248" s="14" t="s">
         <v>1055</v>
       </c>
       <c r="B248" s="9" t="s">
@@ -23741,7 +23731,7 @@
       </c>
     </row>
     <row r="249" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A249" s="15" t="s">
+      <c r="A249" s="14" t="s">
         <v>1057</v>
       </c>
       <c r="B249" s="9" t="s">
@@ -23780,7 +23770,7 @@
       </c>
     </row>
     <row r="250" spans="1:13" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A250" s="15" t="s">
+      <c r="A250" s="14" t="s">
         <v>1059</v>
       </c>
       <c r="B250" s="9" t="s">
@@ -23819,7 +23809,7 @@
       </c>
     </row>
     <row r="251" spans="1:13" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A251" s="15" t="s">
+      <c r="A251" s="14" t="s">
         <v>1061</v>
       </c>
       <c r="B251" s="9" t="s">
@@ -23858,7 +23848,7 @@
       </c>
     </row>
     <row r="252" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A252" s="15" t="s">
+      <c r="A252" s="14" t="s">
         <v>1063</v>
       </c>
       <c r="B252" s="9" t="s">
@@ -23897,7 +23887,7 @@
       </c>
     </row>
     <row r="253" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A253" s="15" t="s">
+      <c r="A253" s="14" t="s">
         <v>1064</v>
       </c>
       <c r="B253" s="9" t="s">
@@ -23936,7 +23926,7 @@
       </c>
     </row>
     <row r="254" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A254" s="15" t="s">
+      <c r="A254" s="14" t="s">
         <v>1065</v>
       </c>
       <c r="B254" s="9" t="s">
@@ -23975,7 +23965,7 @@
       </c>
     </row>
     <row r="255" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A255" s="15" t="s">
+      <c r="A255" s="14" t="s">
         <v>1067</v>
       </c>
       <c r="B255" s="9" t="s">
@@ -24014,7 +24004,7 @@
       </c>
     </row>
     <row r="256" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A256" s="15" t="s">
+      <c r="A256" s="14" t="s">
         <v>1068</v>
       </c>
       <c r="B256" s="9" t="s">
@@ -24053,7 +24043,7 @@
       </c>
     </row>
     <row r="257" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A257" s="15" t="s">
+      <c r="A257" s="14" t="s">
         <v>1070</v>
       </c>
       <c r="B257" s="9" t="s">
@@ -24092,7 +24082,7 @@
       </c>
     </row>
     <row r="258" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A258" s="15" t="s">
+      <c r="A258" s="14" t="s">
         <v>1072</v>
       </c>
       <c r="B258" s="9" t="s">
@@ -24131,7 +24121,7 @@
       </c>
     </row>
     <row r="259" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A259" s="15" t="s">
+      <c r="A259" s="14" t="s">
         <v>205</v>
       </c>
       <c r="B259" s="9" t="s">
@@ -24170,7 +24160,7 @@
       </c>
     </row>
     <row r="260" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A260" s="15" t="s">
+      <c r="A260" s="14" t="s">
         <v>1075</v>
       </c>
       <c r="B260" s="9" t="s">
@@ -24209,7 +24199,7 @@
       </c>
     </row>
     <row r="261" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A261" s="15" t="s">
+      <c r="A261" s="14" t="s">
         <v>1077</v>
       </c>
       <c r="B261" s="9" t="s">
@@ -24248,7 +24238,7 @@
       </c>
     </row>
     <row r="262" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A262" s="15" t="s">
+      <c r="A262" s="14" t="s">
         <v>1079</v>
       </c>
       <c r="B262" s="9" t="s">
@@ -24287,7 +24277,7 @@
       </c>
     </row>
     <row r="263" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A263" s="15" t="s">
+      <c r="A263" s="14" t="s">
         <v>1080</v>
       </c>
       <c r="B263" s="9" t="s">
@@ -24326,7 +24316,7 @@
       </c>
     </row>
     <row r="264" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A264" s="15" t="s">
+      <c r="A264" s="14" t="s">
         <v>1081</v>
       </c>
       <c r="B264" s="9" t="s">
@@ -24365,7 +24355,7 @@
       </c>
     </row>
     <row r="265" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A265" s="15" t="s">
+      <c r="A265" s="14" t="s">
         <v>1082</v>
       </c>
       <c r="B265" s="9" t="s">
@@ -24404,7 +24394,7 @@
       </c>
     </row>
     <row r="266" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A266" s="15" t="s">
+      <c r="A266" s="14" t="s">
         <v>1084</v>
       </c>
       <c r="B266" s="9" t="s">
@@ -24443,7 +24433,7 @@
       </c>
     </row>
     <row r="267" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A267" s="15" t="s">
+      <c r="A267" s="14" t="s">
         <v>1086</v>
       </c>
       <c r="B267" s="9" t="s">
@@ -24482,7 +24472,7 @@
       </c>
     </row>
     <row r="268" spans="1:13" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A268" s="15" t="s">
+      <c r="A268" s="14" t="s">
         <v>1088</v>
       </c>
       <c r="B268" s="9" t="s">
@@ -24521,7 +24511,7 @@
       </c>
     </row>
     <row r="269" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A269" s="15" t="s">
+      <c r="A269" s="14" t="s">
         <v>1090</v>
       </c>
       <c r="B269" s="9" t="s">
@@ -24560,7 +24550,7 @@
       </c>
     </row>
     <row r="270" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A270" s="15" t="s">
+      <c r="A270" s="14" t="s">
         <v>1092</v>
       </c>
       <c r="B270" s="9" t="s">
@@ -24599,7 +24589,7 @@
       </c>
     </row>
     <row r="271" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A271" s="15" t="s">
+      <c r="A271" s="14" t="s">
         <v>1094</v>
       </c>
       <c r="B271" s="9" t="s">
@@ -24638,7 +24628,7 @@
       </c>
     </row>
     <row r="272" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A272" s="15" t="s">
+      <c r="A272" s="14" t="s">
         <v>1096</v>
       </c>
       <c r="B272" s="9" t="s">
@@ -24677,7 +24667,7 @@
       </c>
     </row>
     <row r="273" spans="1:13" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A273" s="15" t="s">
+      <c r="A273" s="14" t="s">
         <v>1098</v>
       </c>
       <c r="B273" s="9" t="s">
@@ -24716,7 +24706,7 @@
       </c>
     </row>
     <row r="274" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A274" s="15" t="s">
+      <c r="A274" s="14" t="s">
         <v>1100</v>
       </c>
       <c r="B274" s="9" t="s">
@@ -24755,7 +24745,7 @@
       </c>
     </row>
     <row r="275" spans="1:13" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A275" s="15" t="s">
+      <c r="A275" s="14" t="s">
         <v>1102</v>
       </c>
       <c r="B275" s="9" t="s">
@@ -24794,7 +24784,7 @@
       </c>
     </row>
     <row r="276" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A276" s="15" t="s">
+      <c r="A276" s="14" t="s">
         <v>1104</v>
       </c>
       <c r="B276" s="9" t="s">
@@ -24833,7 +24823,7 @@
       </c>
     </row>
     <row r="277" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A277" s="15" t="s">
+      <c r="A277" s="14" t="s">
         <v>1106</v>
       </c>
       <c r="B277" s="9" t="s">
@@ -24872,7 +24862,7 @@
       </c>
     </row>
     <row r="278" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A278" s="15" t="s">
+      <c r="A278" s="14" t="s">
         <v>1108</v>
       </c>
       <c r="B278" s="9" t="s">
@@ -24911,7 +24901,7 @@
       </c>
     </row>
     <row r="279" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A279" s="15" t="s">
+      <c r="A279" s="14" t="s">
         <v>1110</v>
       </c>
       <c r="B279" s="9" t="s">
@@ -24950,7 +24940,7 @@
       </c>
     </row>
     <row r="280" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A280" s="15" t="s">
+      <c r="A280" s="14" t="s">
         <v>1112</v>
       </c>
       <c r="B280" s="9" t="s">
@@ -24989,7 +24979,7 @@
       </c>
     </row>
     <row r="281" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A281" s="15" t="s">
+      <c r="A281" s="14" t="s">
         <v>1114</v>
       </c>
       <c r="B281" s="9" t="s">
@@ -25028,7 +25018,7 @@
       </c>
     </row>
     <row r="282" spans="1:13" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A282" s="15" t="s">
+      <c r="A282" s="14" t="s">
         <v>1116</v>
       </c>
       <c r="B282" s="9" t="s">
@@ -25067,7 +25057,7 @@
       </c>
     </row>
     <row r="283" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A283" s="15" t="s">
+      <c r="A283" s="14" t="s">
         <v>1118</v>
       </c>
       <c r="B283" s="9" t="s">
@@ -25106,7 +25096,7 @@
       </c>
     </row>
     <row r="284" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A284" s="15" t="s">
+      <c r="A284" s="14" t="s">
         <v>1120</v>
       </c>
       <c r="B284" s="9" t="s">
@@ -25145,7 +25135,7 @@
       </c>
     </row>
     <row r="285" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A285" s="15" t="s">
+      <c r="A285" s="14" t="s">
         <v>1122</v>
       </c>
       <c r="B285" s="9" t="s">
@@ -25184,7 +25174,7 @@
       </c>
     </row>
     <row r="286" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A286" s="15" t="s">
+      <c r="A286" s="14" t="s">
         <v>1124</v>
       </c>
       <c r="B286" s="9" t="s">
@@ -25223,7 +25213,7 @@
       </c>
     </row>
     <row r="287" spans="1:13" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A287" s="15" t="s">
+      <c r="A287" s="14" t="s">
         <v>1126</v>
       </c>
       <c r="B287" s="9" t="s">
@@ -25262,7 +25252,7 @@
       </c>
     </row>
     <row r="288" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A288" s="15" t="s">
+      <c r="A288" s="14" t="s">
         <v>1128</v>
       </c>
       <c r="B288" s="9" t="s">
@@ -25301,7 +25291,7 @@
       </c>
     </row>
     <row r="289" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A289" s="15" t="s">
+      <c r="A289" s="14" t="s">
         <v>230</v>
       </c>
       <c r="B289" s="9" t="s">
@@ -25340,7 +25330,7 @@
       </c>
     </row>
     <row r="290" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A290" s="15" t="s">
+      <c r="A290" s="14" t="s">
         <v>1129</v>
       </c>
       <c r="B290" s="9" t="s">
@@ -25379,7 +25369,7 @@
       </c>
     </row>
     <row r="291" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A291" s="15" t="s">
+      <c r="A291" s="14" t="s">
         <v>231</v>
       </c>
       <c r="B291" s="9" t="s">
@@ -25418,7 +25408,7 @@
       </c>
     </row>
     <row r="292" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A292" s="15" t="s">
+      <c r="A292" s="14" t="s">
         <v>1132</v>
       </c>
       <c r="B292" s="9" t="s">
@@ -25457,7 +25447,7 @@
       </c>
     </row>
     <row r="293" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A293" s="15" t="s">
+      <c r="A293" s="14" t="s">
         <v>232</v>
       </c>
       <c r="B293" s="9" t="s">
@@ -25496,7 +25486,7 @@
       </c>
     </row>
     <row r="294" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A294" s="15" t="s">
+      <c r="A294" s="14" t="s">
         <v>240</v>
       </c>
       <c r="B294" s="9" t="s">
@@ -25535,7 +25525,7 @@
       </c>
     </row>
     <row r="295" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A295" s="15" t="s">
+      <c r="A295" s="14" t="s">
         <v>1135</v>
       </c>
       <c r="B295" s="9" t="s">
@@ -25574,7 +25564,7 @@
       </c>
     </row>
     <row r="296" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A296" s="15" t="s">
+      <c r="A296" s="14" t="s">
         <v>241</v>
       </c>
       <c r="B296" s="9" t="s">
@@ -25613,7 +25603,7 @@
       </c>
     </row>
     <row r="297" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A297" s="15" t="s">
+      <c r="A297" s="14" t="s">
         <v>1137</v>
       </c>
       <c r="B297" s="9" t="s">
@@ -25652,7 +25642,7 @@
       </c>
     </row>
     <row r="298" spans="1:13" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A298" s="15" t="s">
+      <c r="A298" s="14" t="s">
         <v>1139</v>
       </c>
       <c r="B298" s="9" t="s">
@@ -25691,7 +25681,7 @@
       </c>
     </row>
     <row r="299" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A299" s="15" t="s">
+      <c r="A299" s="14" t="s">
         <v>1141</v>
       </c>
       <c r="B299" s="9" t="s">
@@ -25730,7 +25720,7 @@
       </c>
     </row>
     <row r="300" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A300" s="15" t="s">
+      <c r="A300" s="14" t="s">
         <v>242</v>
       </c>
       <c r="B300" s="9" t="s">
@@ -25769,7 +25759,7 @@
       </c>
     </row>
     <row r="301" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A301" s="15" t="s">
+      <c r="A301" s="14" t="s">
         <v>1143</v>
       </c>
       <c r="B301" s="9" t="s">
@@ -25808,7 +25798,7 @@
       </c>
     </row>
     <row r="302" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A302" s="15" t="s">
+      <c r="A302" s="14" t="s">
         <v>1145</v>
       </c>
       <c r="B302" s="9" t="s">
@@ -25847,7 +25837,7 @@
       </c>
     </row>
     <row r="303" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A303" s="15" t="s">
+      <c r="A303" s="14" t="s">
         <v>243</v>
       </c>
       <c r="B303" s="9" t="s">
@@ -25886,7 +25876,7 @@
       </c>
     </row>
     <row r="304" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A304" s="15" t="s">
+      <c r="A304" s="14" t="s">
         <v>244</v>
       </c>
       <c r="B304" s="9" t="s">
@@ -25925,7 +25915,7 @@
       </c>
     </row>
     <row r="305" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A305" s="15" t="s">
+      <c r="A305" s="14" t="s">
         <v>1148</v>
       </c>
       <c r="B305" s="9" t="s">
@@ -25964,7 +25954,7 @@
       </c>
     </row>
     <row r="306" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A306" s="15" t="s">
+      <c r="A306" s="14" t="s">
         <v>1149</v>
       </c>
       <c r="B306" s="9" t="s">
@@ -26003,7 +25993,7 @@
       </c>
     </row>
     <row r="307" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A307" s="15" t="s">
+      <c r="A307" s="14" t="s">
         <v>1151</v>
       </c>
       <c r="B307" s="9" t="s">
@@ -26042,7 +26032,7 @@
       </c>
     </row>
     <row r="308" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A308" s="15" t="s">
+      <c r="A308" s="14" t="s">
         <v>1152</v>
       </c>
       <c r="B308" s="9" t="s">
@@ -26081,7 +26071,7 @@
       </c>
     </row>
     <row r="309" spans="1:13" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A309" s="15" t="s">
+      <c r="A309" s="14" t="s">
         <v>1153</v>
       </c>
       <c r="B309" s="9" t="s">
@@ -26120,7 +26110,7 @@
       </c>
     </row>
     <row r="310" spans="1:13" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A310" s="15" t="s">
+      <c r="A310" s="14" t="s">
         <v>1155</v>
       </c>
       <c r="B310" s="9" t="s">
@@ -26159,7 +26149,7 @@
       </c>
     </row>
     <row r="311" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A311" s="15"/>
+      <c r="A311" s="14"/>
       <c r="B311" s="9"/>
       <c r="C311" s="5"/>
       <c r="D311" s="8"/>
@@ -26174,7 +26164,7 @@
       <c r="M311" s="8"/>
     </row>
     <row r="312" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A312" s="15"/>
+      <c r="A312" s="14"/>
       <c r="B312" s="9"/>
       <c r="C312" s="5"/>
       <c r="D312" s="8"/>
@@ -26189,7 +26179,7 @@
       <c r="M312" s="8"/>
     </row>
     <row r="313" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A313" s="15"/>
+      <c r="A313" s="14"/>
       <c r="B313" s="9"/>
       <c r="C313" s="5"/>
       <c r="D313" s="8"/>
@@ -26204,7 +26194,7 @@
       <c r="M313" s="8"/>
     </row>
     <row r="314" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A314" s="15"/>
+      <c r="A314" s="14"/>
       <c r="B314" s="9"/>
       <c r="C314" s="5"/>
       <c r="D314" s="8"/>
@@ -26219,7 +26209,7 @@
       <c r="M314" s="8"/>
     </row>
     <row r="315" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A315" s="15"/>
+      <c r="A315" s="14"/>
       <c r="B315" s="9"/>
       <c r="C315" s="5"/>
       <c r="D315" s="8"/>
@@ -26234,7 +26224,7 @@
       <c r="M315" s="8"/>
     </row>
     <row r="316" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A316" s="15"/>
+      <c r="A316" s="14"/>
       <c r="B316" s="9"/>
       <c r="C316" s="5"/>
       <c r="D316" s="8"/>
@@ -26249,7 +26239,7 @@
       <c r="M316" s="8"/>
     </row>
     <row r="317" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A317" s="15"/>
+      <c r="A317" s="14"/>
       <c r="B317" s="9"/>
       <c r="C317" s="5"/>
       <c r="D317" s="8"/>
@@ -26264,7 +26254,7 @@
       <c r="M317" s="8"/>
     </row>
     <row r="318" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A318" s="15"/>
+      <c r="A318" s="14"/>
       <c r="B318" s="9"/>
       <c r="C318" s="5"/>
       <c r="D318" s="8"/>
@@ -26279,7 +26269,7 @@
       <c r="M318" s="8"/>
     </row>
     <row r="319" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A319" s="15"/>
+      <c r="A319" s="14"/>
       <c r="B319" s="9"/>
       <c r="C319" s="5"/>
       <c r="D319" s="8"/>
@@ -26294,7 +26284,7 @@
       <c r="M319" s="8"/>
     </row>
     <row r="320" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A320" s="15"/>
+      <c r="A320" s="14"/>
       <c r="B320" s="9"/>
       <c r="C320" s="5"/>
       <c r="D320" s="8"/>
@@ -26309,7 +26299,7 @@
       <c r="M320" s="8"/>
     </row>
     <row r="321" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A321" s="15"/>
+      <c r="A321" s="14"/>
       <c r="B321" s="9"/>
       <c r="C321" s="5"/>
       <c r="D321" s="8"/>
@@ -26324,7 +26314,7 @@
       <c r="M321" s="8"/>
     </row>
     <row r="322" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A322" s="15"/>
+      <c r="A322" s="14"/>
       <c r="B322" s="9"/>
       <c r="C322" s="5"/>
       <c r="D322" s="8"/>
@@ -26339,7 +26329,7 @@
       <c r="M322" s="8"/>
     </row>
     <row r="323" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A323" s="15"/>
+      <c r="A323" s="14"/>
       <c r="B323" s="9"/>
       <c r="C323" s="5"/>
       <c r="D323" s="8"/>
@@ -26354,7 +26344,7 @@
       <c r="M323" s="8"/>
     </row>
     <row r="324" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A324" s="15"/>
+      <c r="A324" s="14"/>
       <c r="B324" s="9"/>
       <c r="C324" s="5"/>
       <c r="D324" s="8"/>
@@ -26369,7 +26359,7 @@
       <c r="M324" s="8"/>
     </row>
     <row r="325" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A325" s="15"/>
+      <c r="A325" s="14"/>
       <c r="B325" s="9"/>
       <c r="C325" s="5"/>
       <c r="D325" s="8"/>

</xml_diff>